<commit_message>
Mise a jour du mini prototype
</commit_message>
<xml_diff>
--- a/mini-rag-ui/data/documents/table.xlsx
+++ b/mini-rag-ui/data/documents/table.xlsx
@@ -34,7 +34,7 @@
     <t>Backend Dev</t>
   </si>
   <si>
-    <t>Python / FastAPI</t>
+    <t>Python/FastAPI</t>
   </si>
   <si>
     <t>JobMatchAI</t>
@@ -58,7 +58,7 @@
     <t>Data Engineer</t>
   </si>
   <si>
-    <t>Python / ML</t>
+    <t>Python/ML</t>
   </si>
   <si>
     <t>SmartAI</t>
@@ -70,7 +70,7 @@
     <t>DevOps</t>
   </si>
   <si>
-    <t>Docker / AWS</t>
+    <t>Docker/AWS</t>
   </si>
   <si>
     <t>InfraCloud</t>
@@ -98,7 +98,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -142,7 +142,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="31.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33" customFormat="1" s="1">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="31.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33" customFormat="1" s="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -500,7 +500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -514,7 +514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>

</xml_diff>